<commit_message>
added summary tab to make a chart
</commit_message>
<xml_diff>
--- a/paper/Content Inventory.xlsx
+++ b/paper/Content Inventory.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -79,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="349">
   <si>
     <t>Notes</t>
   </si>
@@ -1210,6 +1211,18 @@
   </si>
   <si>
     <t>EZProxy prepend on database URLS</t>
+  </si>
+  <si>
+    <t>Total number of pages</t>
+  </si>
+  <si>
+    <t>Pages with less than 1% view rate</t>
+  </si>
+  <si>
+    <t>Pages with more than 1% view rate</t>
+  </si>
+  <si>
+    <t>Pages with no data</t>
   </si>
 </sst>
 </file>
@@ -1374,6 +1387,820 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Percentage</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> of Pageviews for library.iit.edu </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Pages with more than 1% view rate</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pages with less than 1% view rate</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pages with no data</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$B$2:$D$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1465,6 +2292,41 @@
         </a:ln>
       </xdr:spPr>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>128586</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>333374</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1735,9 +2597,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB218"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -4978,4 +5840,51 @@
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>107</v>
+      </c>
+      <c r="B2">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>61</v>
+      </c>
+      <c r="D2">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding additional citations and examples
</commit_message>
<xml_diff>
--- a/paper/Content Inventory.xlsx
+++ b/paper/Content Inventory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -2597,9 +2597,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB218"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A108" sqref="A108"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -5846,7 +5846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
sorted and made content inventory a pdf
</commit_message>
<xml_diff>
--- a/paper/Content Inventory.xlsx
+++ b/paper/Content Inventory.xlsx
@@ -16,6 +16,8 @@
     <sheet name="Summary" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Inventory!$A$1:$G$105</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Inventory!$1:$1</definedName>
     <definedName name="StaticItemNumbers">#REF!</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -1346,7 +1348,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1486,7 +1487,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2413,8 +2413,8 @@
   <dimension ref="A1:G105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2423,8 +2423,8 @@
     <col min="2" max="2" width="17.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="22.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="17.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="36.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="45.42578125" style="3" customWidth="1"/>
     <col min="7" max="7" width="40.42578125" style="3" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
@@ -2454,1761 +2454,1755 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.2039</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>27</v>
+        <v>9</v>
+      </c>
+      <c r="D3" s="4">
+        <v>4.9700000000000001E-2</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>36</v>
+        <v>12</v>
+      </c>
+      <c r="D4" s="4">
+        <v>4.1300000000000003E-2</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="F5" s="3" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="4">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>28</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>29</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>140</v>
+        <v>31</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>141</v>
+        <v>32</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>158</v>
+        <v>35</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>159</v>
+        <v>36</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>160</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>165</v>
+        <v>38</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>166</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
-        <v>54</v>
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>27</v>
+        <v>41</v>
+      </c>
+      <c r="D12" s="4">
+        <v>2.01E-2</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>168</v>
+        <v>42</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>169</v>
+        <v>43</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>64</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <v>65</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
-        <v>67</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>197</v>
+        <v>15</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>27</v>
+        <v>56</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1E-4</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>208</v>
+        <v>57</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
-        <v>75</v>
+        <v>17</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>228</v>
+        <v>59</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>229</v>
+        <v>60</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
-        <v>83</v>
+        <v>22</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>27</v>
+        <v>62</v>
+      </c>
+      <c r="D18" s="4">
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>256</v>
+        <v>63</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>257</v>
+        <v>64</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
-        <v>86</v>
+        <v>23</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>27</v>
+        <v>67</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1.6999999999999999E-3</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>264</v>
+        <v>68</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
-        <v>88</v>
+        <v>24</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>27</v>
+        <v>71</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>271</v>
+        <v>72</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>272</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
-        <v>89</v>
+        <v>25</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>27</v>
+        <v>74</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>274</v>
+        <v>75</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>275</v>
+        <v>76</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>278</v>
+        <v>78</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>283</v>
+        <v>34</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>27</v>
+        <v>80</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>303</v>
+        <v>81</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>305</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>306</v>
+        <v>83</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>307</v>
+        <v>84</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>309</v>
+        <v>86</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>310</v>
+        <v>87</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
-        <v>103</v>
+        <v>30</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>27</v>
+        <v>89</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1E-4</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>314</v>
+        <v>90</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>315</v>
+        <v>91</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
-        <v>105</v>
+        <v>31</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>27</v>
+        <v>93</v>
+      </c>
+      <c r="D27" s="4">
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>321</v>
+        <v>94</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>322</v>
+        <v>95</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
-        <v>106</v>
+        <v>32</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>27</v>
+        <v>66</v>
+      </c>
+      <c r="D28" s="4">
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>324</v>
+        <v>97</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
-        <v>107</v>
+        <v>33</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>27</v>
+      <c r="D29" s="4">
+        <v>3.0999999999999999E-3</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>326</v>
+        <v>92</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>327</v>
+        <v>100</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
-        <v>108</v>
+        <v>34</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="D30" s="4">
+        <v>1.4E-3</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>330</v>
+        <v>102</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>331</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
+        <v>35</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1.9800000000000002E-2</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>36</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
-        <v>60</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>27</v>
+      <c r="D32" s="4">
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>345</v>
+        <v>110</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>346</v>
+        <v>111</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
-        <v>14</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>354</v>
+        <v>37</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>13</v>
+        <v>113</v>
+      </c>
+      <c r="D33" s="4">
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
-        <v>62</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>188</v>
+        <v>38</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>13</v>
+        <v>116</v>
+      </c>
+      <c r="D34" s="4">
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>190</v>
+        <v>117</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="D35" s="4">
-        <v>0.2039</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>7</v>
+        <v>121</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
-        <v>41</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="D36" s="4">
-        <v>5.2499999999999998E-2</v>
+        <v>2.63E-2</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>9</v>
+        <v>125</v>
       </c>
       <c r="D37" s="4">
-        <v>4.9700000000000001E-2</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>10</v>
+        <v>126</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>12</v>
+        <v>129</v>
       </c>
       <c r="D38" s="4">
-        <v>4.1300000000000003E-2</v>
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="178.5" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="D39" s="4">
-        <v>2.63E-2</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>38</v>
+        <v>135</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
       <c r="D40" s="4">
-        <v>2.1000000000000001E-2</v>
+        <v>1.9E-3</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
-        <v>57</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>176</v>
+        <v>45</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="D41" s="4">
-        <v>2.0299999999999999E-2</v>
+        <v>140</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>178</v>
+        <v>141</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>180</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
-        <v>11</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>41</v>
+        <v>143</v>
       </c>
       <c r="D42" s="4">
-        <v>2.01E-2</v>
+        <v>1E-4</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>42</v>
+        <v>144</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>105</v>
+        <v>146</v>
       </c>
       <c r="D43" s="4">
-        <v>1.9800000000000002E-2</v>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>106</v>
+        <v>147</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>218</v>
+        <v>149</v>
       </c>
       <c r="D44" s="4">
-        <v>8.8999999999999999E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>219</v>
+        <v>150</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="D45" s="4">
-        <v>6.6E-3</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>185</v>
+        <v>153</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>187</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
-        <v>12</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>349</v>
+        <v>50</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>45</v>
+        <v>155</v>
       </c>
       <c r="D46" s="4">
-        <v>5.0000000000000001E-3</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>46</v>
+        <v>156</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>48</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
-        <v>98</v>
-      </c>
-      <c r="D47" s="4">
-        <v>4.1000000000000003E-3</v>
+        <v>51</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>38</v>
+        <v>159</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
-        <v>113</v>
+        <v>52</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>231</v>
+        <v>161</v>
       </c>
       <c r="D48" s="4">
-        <v>3.3999999999999998E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>341</v>
+        <v>162</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>343</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="D49" s="4">
-        <v>3.3E-3</v>
+        <v>164</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>226</v>
+        <v>165</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>227</v>
+        <v>166</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D50" s="4">
-        <v>3.0999999999999999E-3</v>
+        <v>167</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>92</v>
+        <v>168</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
-        <v>63</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D51" s="4">
-        <v>3.0999999999999999E-3</v>
+        <v>170</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
-        <v>81</v>
+        <v>56</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="D52" s="4">
-        <v>3.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>38</v>
+        <v>173</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>249</v>
+        <v>174</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>288</v>
+        <v>176</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>289</v>
+        <v>177</v>
       </c>
       <c r="D53" s="4">
-        <v>2.8E-3</v>
+        <v>2.0299999999999999E-2</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>290</v>
+        <v>178</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>291</v>
+        <v>179</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>292</v>
+        <v>180</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>129</v>
+        <v>181</v>
       </c>
       <c r="D54" s="4">
-        <v>2.7000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>130</v>
+        <v>182</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>131</v>
+        <v>183</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="216.75" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D55" s="4">
-        <v>2E-3</v>
+        <v>344</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>173</v>
+        <v>345</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>174</v>
+        <v>346</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>137</v>
+        <v>104</v>
       </c>
       <c r="D56" s="4">
-        <v>1.9E-3</v>
+        <v>6.6E-3</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>138</v>
+        <v>185</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
-        <v>23</v>
+        <v>62</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="C57" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A58" s="3">
+        <v>63</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D58" s="4">
+        <v>3.0999999999999999E-3</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A59" s="3">
+        <v>64</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A60" s="3">
+        <v>65</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A61" s="3">
+        <v>66</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D61" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A62" s="3">
         <v>67</v>
       </c>
-      <c r="D57" s="4">
-        <v>1.6999999999999999E-3</v>
-      </c>
-      <c r="E57" s="5" t="s">
+      <c r="B62" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A63" s="3">
         <v>68</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="D63" s="4">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A64" s="3">
         <v>69</v>
       </c>
-      <c r="G57" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="3">
-        <v>34</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D58" s="4">
-        <v>1.4E-3</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A59" s="3">
-        <v>76</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D59" s="4">
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A60" s="3">
-        <v>90</v>
-      </c>
-      <c r="D60" s="4">
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A61" s="3">
-        <v>24</v>
-      </c>
-      <c r="C61" s="3" t="s">
+      <c r="C64" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D64" s="4">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A65" s="3">
         <v>71</v>
       </c>
-      <c r="D61" s="4">
+      <c r="C65" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D65" s="4">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="E61" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A62" s="3">
-        <v>43</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D62" s="4">
-        <v>1.1000000000000001E-3</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A63" s="3">
-        <v>71</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="D63" s="4">
-        <v>1.1000000000000001E-3</v>
-      </c>
-      <c r="E63" s="5" t="s">
+      <c r="E65" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="F63" s="3" t="s">
+      <c r="F65" s="3" t="s">
         <v>217</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A64" s="3">
-        <v>6</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D64" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A65" s="3">
-        <v>13</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D65" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
+        <v>72</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D66" s="4">
+        <v>8.8999999999999999E-3</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A67" s="3">
         <v>73</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C67" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="D66" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A67" s="3">
-        <v>59</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>181</v>
       </c>
       <c r="D67" s="4">
         <v>1E-3</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>182</v>
+        <v>223</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>183</v>
+        <v>224</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>116</v>
+        <v>193</v>
       </c>
       <c r="D68" s="4">
-        <v>8.9999999999999998E-4</v>
+        <v>3.3E-3</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>117</v>
+        <v>226</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
-        <v>68</v>
-      </c>
-      <c r="D69" s="4">
-        <v>8.9999999999999998E-4</v>
+        <v>75</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>38</v>
+        <v>229</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="D70" s="4">
-        <v>8.9999999999999998E-4</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>62</v>
+        <v>235</v>
       </c>
       <c r="D71" s="4">
-        <v>8.0000000000000004E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>63</v>
+        <v>236</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G71" s="3" t="s">
-        <v>65</v>
+        <v>237</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
-        <v>32</v>
+        <v>78</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>66</v>
+        <v>238</v>
       </c>
       <c r="D72" s="4">
-        <v>8.0000000000000004E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>97</v>
+        <v>239</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>120</v>
+        <v>241</v>
       </c>
       <c r="D73" s="4">
-        <v>8.0000000000000004E-4</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>121</v>
+        <v>242</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
-        <v>112</v>
+        <v>80</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>244</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>297</v>
+        <v>245</v>
       </c>
       <c r="D74" s="4">
-        <v>8.0000000000000004E-4</v>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>339</v>
+        <v>246</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
-        <v>47</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>146</v>
+        <v>81</v>
       </c>
       <c r="D75" s="4">
-        <v>6.9999999999999999E-4</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
-        <v>80</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>244</v>
+        <v>82</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="D76" s="4">
-        <v>6.9999999999999999E-4</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
-        <v>37</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D77" s="4">
-        <v>5.9999999999999995E-4</v>
+        <v>255</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>114</v>
+        <v>256</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>211</v>
+        <v>258</v>
       </c>
       <c r="D78" s="4">
-        <v>5.9999999999999995E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>212</v>
+        <v>259</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>213</v>
+        <v>260</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
-        <v>4</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="D79" s="4">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
-        <v>85</v>
-      </c>
-      <c r="D80" s="4">
-        <v>5.0000000000000001E-4</v>
+        <v>86</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>38</v>
+        <v>264</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="G80" s="3" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
-        <v>95</v>
+        <v>87</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>266</v>
       </c>
       <c r="D81" s="4">
-        <v>5.0000000000000001E-4</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>38</v>
+        <v>267</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>287</v>
+        <v>268</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>195</v>
+        <v>269</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
-        <v>5</v>
+        <v>88</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D82" s="4">
-        <v>4.0000000000000002E-4</v>
+        <v>270</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>20</v>
+        <v>271</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>21</v>
+        <v>272</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="D83" s="4">
-        <v>4.0000000000000002E-4</v>
+        <v>273</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>294</v>
+        <v>274</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="G83" s="3" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
-        <v>99</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>298</v>
+        <v>90</v>
       </c>
       <c r="D84" s="4">
-        <v>4.0000000000000002E-4</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>299</v>
+        <v>38</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>300</v>
+        <v>276</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>301</v>
+        <v>277</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>74</v>
+        <v>279</v>
       </c>
       <c r="D85" s="4">
-        <v>2.9999999999999997E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>75</v>
+        <v>280</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>76</v>
+        <v>281</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="D86" s="4">
-        <v>2.9999999999999997E-4</v>
+        <v>278</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>156</v>
+        <v>282</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+        <v>283</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="D87" s="4">
-        <v>2.9999999999999997E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>252</v>
+        <v>285</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>253</v>
+        <v>286</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
-        <v>87</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>266</v>
+        <v>95</v>
       </c>
       <c r="D88" s="4">
-        <v>2.9999999999999997E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>267</v>
+        <v>38</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
-        <v>10</v>
+        <v>96</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>288</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>30</v>
+        <v>289</v>
       </c>
       <c r="D89" s="4">
-        <v>2.0000000000000001E-4</v>
+        <v>2.8E-3</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>38</v>
+        <v>290</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>39</v>
+        <v>291</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>80</v>
+        <v>293</v>
       </c>
       <c r="D90" s="4">
-        <v>2.0000000000000001E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>81</v>
+        <v>294</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>82</v>
+        <v>295</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
-        <v>31</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D91" s="4">
-        <v>2.0000000000000001E-4</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G91" s="3" t="s">
-        <v>96</v>
+        <v>296</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>152</v>
+        <v>298</v>
       </c>
       <c r="D92" s="4">
-        <v>2.0000000000000001E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>153</v>
+        <v>299</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
+        <v>100</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A94" s="3">
+        <v>101</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A95" s="3">
+        <v>102</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A96" s="3">
+        <v>103</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="G96" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="D93" s="4">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="E93" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="F93" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A94" s="3">
-        <v>78</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="D94" s="4">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="E94" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="F94" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A95" s="3">
-        <v>84</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D95" s="4">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="E95" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="F95" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="G95" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A96" s="3">
-        <v>94</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="D96" s="4">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="E96" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="F96" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
@@ -4233,154 +4227,161 @@
     </row>
     <row r="98" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="D98" s="4">
-        <v>2.0000000000000001E-4</v>
+        <v>320</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
-        <v>15</v>
+        <v>106</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D99" s="4">
-        <v>1E-4</v>
+        <v>323</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>57</v>
+        <v>324</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+        <v>325</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
-        <v>30</v>
+        <v>107</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D100" s="4">
-        <v>1E-4</v>
+        <v>99</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>90</v>
+        <v>326</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>91</v>
+        <v>327</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>92</v>
+        <v>328</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
-        <v>46</v>
+        <v>108</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D101" s="4">
-        <v>1E-4</v>
+        <v>329</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>144</v>
+        <v>330</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>145</v>
+        <v>331</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
-        <v>48</v>
+        <v>109</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="D102" s="4">
-        <v>1E-4</v>
+        <v>332</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>150</v>
+        <v>333</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>161</v>
+        <v>335</v>
       </c>
       <c r="D103" s="4">
-        <v>1E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>162</v>
+        <v>336</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+        <v>337</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
-        <v>66</v>
+        <v>112</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>204</v>
+        <v>297</v>
       </c>
       <c r="D104" s="4">
-        <v>1E-4</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>205</v>
+        <v>339</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>279</v>
+        <v>231</v>
       </c>
       <c r="D105" s="4">
-        <v>1E-4</v>
+        <v>3.3999999999999998E-3</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>280</v>
+        <v>341</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>281</v>
+        <v>342</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>195</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:G105">
-    <sortCondition descending="1" ref="D2:D105"/>
+    <sortCondition ref="A2:A105"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="17" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>